<commit_message>
[React 16 - 9. Reaching out to the Web (Http  Ajax)]
</commit_message>
<xml_diff>
--- a/reactjs/React 16 - The Complete Guide/Timesheet.xlsx
+++ b/reactjs/React 16 - The Complete Guide/Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vipothamse.COPART\git\docs\reactjs\React 16 - The Complete Guide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC6CEB8-AFD2-4D30-A049-D0C492611315}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37F9CED-E624-4B0F-BF48-071B95C15406}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5985" xr2:uid="{0A474607-024F-417D-B984-B80057D184F8}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="382">
   <si>
     <t>1. Getting Started</t>
   </si>
@@ -1540,8 +1540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{322B2238-9126-4447-A494-5C8BA9F1223A}">
   <dimension ref="A1:L405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D132" sqref="D132:D134"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D134" sqref="D134:D151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3663,6 +3663,9 @@
       <c r="C135" s="3">
         <v>0</v>
       </c>
+      <c r="D135" s="5" t="s">
+        <v>381</v>
+      </c>
       <c r="L135" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3675,6 +3678,9 @@
       <c r="C136" s="3">
         <v>4.3750000000000004E-2</v>
       </c>
+      <c r="D136" s="5" t="s">
+        <v>381</v>
+      </c>
       <c r="K136" s="2">
         <v>63</v>
       </c>
@@ -3690,6 +3696,9 @@
       <c r="C137" s="3">
         <v>6.5972222222222224E-2</v>
       </c>
+      <c r="D137" s="5" t="s">
+        <v>381</v>
+      </c>
       <c r="K137" s="2">
         <v>95</v>
       </c>
@@ -3705,6 +3714,9 @@
       <c r="C138" s="3">
         <v>0.17083333333333331</v>
       </c>
+      <c r="D138" s="5" t="s">
+        <v>381</v>
+      </c>
       <c r="K138" s="2">
         <v>246</v>
       </c>
@@ -3720,6 +3732,9 @@
       <c r="C139" s="3">
         <v>0.22847222222222222</v>
       </c>
+      <c r="D139" s="5" t="s">
+        <v>381</v>
+      </c>
       <c r="K139" s="2">
         <v>329</v>
       </c>
@@ -3735,6 +3750,9 @@
       <c r="C140" s="3">
         <v>0.15694444444444444</v>
       </c>
+      <c r="D140" s="5" t="s">
+        <v>381</v>
+      </c>
       <c r="K140" s="2">
         <v>226</v>
       </c>
@@ -3750,6 +3768,9 @@
       <c r="C141" s="3">
         <v>0.1111111111111111</v>
       </c>
+      <c r="D141" s="5" t="s">
+        <v>381</v>
+      </c>
       <c r="K141" s="2">
         <v>160</v>
       </c>
@@ -3765,6 +3786,9 @@
       <c r="C142" s="3">
         <v>0.1673611111111111</v>
       </c>
+      <c r="D142" s="5" t="s">
+        <v>381</v>
+      </c>
       <c r="K142" s="2">
         <v>241</v>
       </c>
@@ -3780,6 +3804,9 @@
       <c r="C143" s="3">
         <v>0.33055555555555555</v>
       </c>
+      <c r="D143" s="5" t="s">
+        <v>381</v>
+      </c>
       <c r="K143" s="2">
         <v>476</v>
       </c>
@@ -3795,6 +3822,9 @@
       <c r="C144" s="3">
         <v>0.16111111111111112</v>
       </c>
+      <c r="D144" s="5" t="s">
+        <v>381</v>
+      </c>
       <c r="K144" s="2">
         <v>232</v>
       </c>
@@ -3810,6 +3840,9 @@
       <c r="C145" s="3">
         <v>9.930555555555555E-2</v>
       </c>
+      <c r="D145" s="5" t="s">
+        <v>381</v>
+      </c>
       <c r="K145" s="2">
         <v>143</v>
       </c>
@@ -3825,6 +3858,9 @@
       <c r="C146" s="3">
         <v>2.2916666666666669E-2</v>
       </c>
+      <c r="D146" s="5" t="s">
+        <v>381</v>
+      </c>
       <c r="K146" s="2">
         <v>33</v>
       </c>
@@ -3840,6 +3876,9 @@
       <c r="C147" s="3">
         <v>0.14097222222222222</v>
       </c>
+      <c r="D147" s="5" t="s">
+        <v>381</v>
+      </c>
       <c r="K147" s="2">
         <v>203</v>
       </c>
@@ -3855,6 +3894,9 @@
       <c r="C148" s="3">
         <v>0.26250000000000001</v>
       </c>
+      <c r="D148" s="5" t="s">
+        <v>381</v>
+      </c>
       <c r="K148" s="2">
         <v>378</v>
       </c>
@@ -3870,6 +3912,9 @@
       <c r="C149" s="3">
         <v>0.13194444444444445</v>
       </c>
+      <c r="D149" s="5" t="s">
+        <v>381</v>
+      </c>
       <c r="K149" s="2">
         <v>190</v>
       </c>
@@ -3885,6 +3930,9 @@
       <c r="C150" s="3">
         <v>0.21041666666666667</v>
       </c>
+      <c r="D150" s="5" t="s">
+        <v>381</v>
+      </c>
       <c r="K150" s="2">
         <v>303</v>
       </c>
@@ -3899,6 +3947,9 @@
       </c>
       <c r="C151" s="3">
         <v>3.2638888888888891E-2</v>
+      </c>
+      <c r="D151" s="5" t="s">
+        <v>381</v>
       </c>
       <c r="K151" s="2">
         <v>47</v>

</xml_diff>